<commit_message>
weekly task error handling and chagnes
</commit_message>
<xml_diff>
--- a/Base/src/main/resources/templates/format3.xlsx
+++ b/Base/src/main/resources/templates/format3.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Client</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Project Type</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -150,6 +153,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -157,9 +163,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,13 +444,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H281"/>
+  <dimension ref="B1:I281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,93 +462,98 @@
     <col min="5" max="5" width="26.28515625" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" style="1" customWidth="1"/>
+    <col min="8" max="9" width="26.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="2:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="2:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="G16" s="4"/>
     </row>
@@ -1563,59 +1571,23 @@
       <c r="G281" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:WXS3"/>
-  <mergeCells count="7">
+  <autoFilter ref="A3:WXT3"/>
+  <mergeCells count="8">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="H2:H3"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576 C4:D281 G4:I281">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B235:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>G4:G281</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C4:C281</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D4:D281</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4:B234</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>H4:H281</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>